<commit_message>
Fixed BOM and PnP files
</commit_message>
<xml_diff>
--- a/cam/USB2Serial_CH340G_v1.2_2021-04-08-PnP.xlsx
+++ b/cam/USB2Serial_CH340G_v1.2_2021-04-08-PnP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\USB2Serial\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BBF5EF-907F-4115-BFBE-3F03461EC07C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CC59C3-03B4-486F-A4BF-B08B78DF9A73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14130" yWindow="470" windowWidth="20910" windowHeight="20770" activeTab="1" xr2:uid="{5D2895E1-8DCD-4B82-B23D-D97D58D61A28}"/>
+    <workbookView xWindow="17430" yWindow="230" windowWidth="20910" windowHeight="20770" activeTab="1" xr2:uid="{5D2895E1-8DCD-4B82-B23D-D97D58D61A28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,8 +220,8 @@
     <tableColumn id="7" xr3:uid="{DE0E2F91-549F-4893-8570-DCA7E8157B30}" uniqueName="7" name="Designator" queryTableFieldId="1" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{5CE4AE43-7473-4367-9F59-1DB5C744145E}" uniqueName="2" name="Mid X" queryTableFieldId="2" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{B77DCC83-F606-477C-8FAE-23C6DBD234BD}" uniqueName="3" name="Mid Y" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{5FC86AB8-6D45-48E5-918B-8AD8078ED627}" uniqueName="8" name="Layer" queryTableFieldId="7" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{1ECE8D76-6114-4856-841F-6867EFF1E5DD}" uniqueName="4" name="Rotation" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{5FC86AB8-6D45-48E5-918B-8AD8078ED627}" uniqueName="8" name="Layer" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{1ECE8D76-6114-4856-841F-6867EFF1E5DD}" uniqueName="4" name="Rotation" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -539,7 +539,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,7 +734,7 @@
         <v>26</v>
       </c>
       <c r="E11" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>